<commit_message>
fix: removido print do procedimento filtrado
</commit_message>
<xml_diff>
--- a/dados_sisreg.xlsx
+++ b/dados_sisreg.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Cod. Unificado</t>
   </si>
@@ -46,19 +46,28 @@
     <t xml:space="preserve">Municipio</t>
   </si>
   <si>
-    <t xml:space="preserve">0301010072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0001005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSULTA EM CIRURGIA DE CABEÇA E PESCOÇO - GERAL - PPI</t>
+    <t xml:space="preserve">0301130035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0063005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACOLHIMENTO PARA PROCESSO TRANSEXUALIZADOR</t>
   </si>
   <si>
     <t xml:space="preserve">FISICO</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiradentes</t>
+    <t xml:space="preserve">Monsenhor Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0301010048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0724035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSULTA EM DOENÇAS RARAS - TRIAGEM</t>
   </si>
 </sst>
 </file>
@@ -69,7 +78,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -91,26 +100,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,20 +143,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,229 +275,101 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="70.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="92.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.74"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="H33" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>